<commit_message>
Acoustics BOM work and Created board STEP
</commit_message>
<xml_diff>
--- a/TalosBoards/Acoustics/Acoustics BOM.xlsx
+++ b/TalosBoards/Acoustics/Acoustics BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\Everything\UWRT\Electrical\GIT\electric_boogaloo\TempestBoards\Acoustics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\Everything\UWRT\Electrical\GIT\electric_boogaloo\TalosBoards\Acoustics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BE2DD6-7EE6-4CAA-8726-B468F6E92365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE2D8E7-FA71-4F66-8654-32844A768A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="212">
   <si>
     <t>Distributor</t>
   </si>
@@ -663,6 +663,33 @@
   </si>
   <si>
     <t>PE-0402CL470JTT</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>WM13195-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/molex/0353180420/3185063?s=N4IgTCBcDaIOoFkCMBmJBOArAWgHIBEQBdAXyA</t>
+  </si>
+  <si>
+    <t>Minifit jr R/A 4 pin</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/molex/0039300020/930320</t>
+  </si>
+  <si>
+    <t>WM21351-ND</t>
+  </si>
+  <si>
+    <t>Minifit jr R/A 2 pin</t>
+  </si>
+  <si>
+    <t>Weren't listed in the inventory report but we may have some</t>
+  </si>
+  <si>
+    <t>This and the 2 pin below also need their respective connectors</t>
   </si>
 </sst>
 </file>
@@ -815,7 +842,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -868,6 +895,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1167,8 +1200,8 @@
   <dimension ref="B1:M73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2637,103 +2670,151 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="C49" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D49" t="s">
+        <v>204</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F49" s="21">
+        <v>353180420</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H49" s="1">
+        <v>2</v>
+      </c>
+      <c r="I49" s="1">
+        <v>5</v>
+      </c>
       <c r="J49" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="C50" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D50" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F50" s="22">
+        <v>39300020</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="H50" s="1">
+        <v>2</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0</v>
+      </c>
       <c r="J50" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+        <f>I50-H50</f>
+        <v>-2</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J51" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J52" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J53" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J54" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J55" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J56" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J57" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J58" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J59" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J60" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J61" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J62" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J63" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J64" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2847,8 +2928,10 @@
     <hyperlink ref="B20" r:id="rId45" xr:uid="{D8ECC531-137A-47E3-8E7B-7F5B3E16C0DC}"/>
     <hyperlink ref="B47" r:id="rId46" xr:uid="{EC666389-E9C0-49A7-B16D-0DBB03248AC5}"/>
     <hyperlink ref="B48" r:id="rId47" xr:uid="{660ECBA0-88CE-4515-B5E8-18D239CB5FAE}"/>
+    <hyperlink ref="B49" r:id="rId48" xr:uid="{4E4A2185-D8AF-43D1-8D11-24E04B32F50B}"/>
+    <hyperlink ref="B50" r:id="rId49" xr:uid="{771B35E7-FDFB-41F5-B84B-05C74899FB84}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId48"/>
+  <legacyDrawing r:id="rId50"/>
 </worksheet>
 </file>
</xml_diff>